<commit_message>
added save to file
- also fixed goodness scoring
- more minor changes to improve accuracy
</commit_message>
<xml_diff>
--- a/code/js/test/correct answers.xlsx
+++ b/code/js/test/correct answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py\gsa\code\js\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D53E89-A9D0-4499-A6A8-3F80CEB9F0C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFF33F3-AD67-4A81-849A-8B578F3A540C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="3870" windowWidth="12330" windowHeight="15435" xr2:uid="{2E394A29-1AF7-4FAC-A203-4A1F3EB1E0FF}"/>
+    <workbookView xWindow="7245" yWindow="2190" windowWidth="25980" windowHeight="14970" xr2:uid="{2E394A29-1AF7-4FAC-A203-4A1F3EB1E0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Eveningness</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>&lt;1</t>
-  </si>
-  <si>
-    <t>&lt;0</t>
   </si>
 </sst>
 </file>
@@ -489,16 +486,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>